<commit_message>
API - Test flows - base
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/APITests/APITestsTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/APITests/APITestsTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Password</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>SampleTestForApi</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -415,9 +421,14 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="1"/>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
eGov - Create authtoken step checkin
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/APITests/APITestsTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/APITests/APITestsTestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BaseAPITests" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateComplaint" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Password</t>
   </si>
@@ -43,6 +44,12 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>createComplaint</t>
   </si>
 </sst>
 </file>
@@ -382,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -435,4 +442,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All object types - dynamic identification of keys
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/APITests/APITestsTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/APITests/APITestsTestData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BaseAPITests" sheetId="1" r:id="rId1"/>
     <sheet name="CreateComplaint" sheetId="2" r:id="rId2"/>
+    <sheet name="AllObjectTypes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Password</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>createComplaint</t>
+  </si>
+  <si>
+    <t>validateAllObjTypes</t>
   </si>
 </sst>
 </file>
@@ -448,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -473,4 +477,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>